<commit_message>
Desenvolvimento de código para estruturação de pastas e automação do fluxo interno
</commit_message>
<xml_diff>
--- a/portal_blumenau/Parametros_BluBot.xlsx
+++ b/portal_blumenau/Parametros_BluBot.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Matrícula</t>
   </si>
@@ -49,13 +49,7 @@
     <t>Ano final</t>
   </si>
   <si>
-    <t>Caminho para pasta do cliente</t>
-  </si>
-  <si>
     <t>2022</t>
-  </si>
-  <si>
-    <t>.</t>
   </si>
   <si>
     <t>GILMAR BARG</t>
@@ -511,10 +505,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A3" sqref="A3:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,12 +519,11 @@
     <col min="4" max="4" width="10.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.5703125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="8" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="5" hidden="1"/>
+    <col min="7" max="7" width="7.140625" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,35 +540,29 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="D2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -602,70 +589,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>